<commit_message>
Changes to be committed: 	new file:   ta/Correction for TRTS-4S.ipynb 	new file:   "ta/TRTS-4S\345\261\217\346\237\265\347\267\232.xlsx" 	modified:   ta/correction.ipynb 	modified:   "ta/\346\240\241\344\274\260.xlsx"
</commit_message>
<xml_diff>
--- a/ta/校估.xlsx
+++ b/ta/校估.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Allen\Desktop\Traffic-Assignment-Model\ta\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\暫存\Traffic-Assignment-Model\ta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{971ED556-1867-4D98-AC88-FC7676AC335B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA65C52A-45E6-4057-A310-F82D8F2BBA49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{226A0F74-BF97-4CA0-AC08-8509B73241AA}"/>
+    <workbookView xWindow="300" yWindow="2610" windowWidth="21600" windowHeight="11835" activeTab="1" xr2:uid="{226A0F74-BF97-4CA0-AC08-8509B73241AA}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="84">
   <si>
     <t>A</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -368,6 +368,10 @@
   </si>
   <si>
     <t>淡水出</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>S</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -764,16 +768,16 @@
   <dimension ref="A1:G48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>69</v>
       </c>
@@ -793,7 +797,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>81</v>
       </c>
@@ -813,7 +817,7 @@
         <v>10115</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>82</v>
       </c>
@@ -833,7 +837,7 @@
         <v>5854</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>81</v>
       </c>
@@ -853,7 +857,7 @@
         <v>5871</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>82</v>
       </c>
@@ -873,7 +877,7 @@
         <v>5865</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>72</v>
       </c>
@@ -893,7 +897,7 @@
         <v>8115</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>73</v>
       </c>
@@ -914,7 +918,7 @@
       </c>
       <c r="G7" s="1"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>72</v>
       </c>
@@ -934,7 +938,7 @@
         <v>6813</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>73</v>
       </c>
@@ -954,7 +958,7 @@
         <v>8607</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>72</v>
       </c>
@@ -974,7 +978,7 @@
         <v>15667</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>73</v>
       </c>
@@ -994,7 +998,7 @@
         <v>8289</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>78</v>
       </c>
@@ -1014,7 +1018,7 @@
         <v>10265</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>72</v>
       </c>
@@ -1034,7 +1038,7 @@
         <v>8343</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>73</v>
       </c>
@@ -1054,7 +1058,7 @@
         <v>6675</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>72</v>
       </c>
@@ -1074,7 +1078,7 @@
         <v>27271</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>73</v>
       </c>
@@ -1094,7 +1098,7 @@
         <v>6675</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>74</v>
       </c>
@@ -1114,7 +1118,7 @@
         <v>6760</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>75</v>
       </c>
@@ -1134,7 +1138,7 @@
         <v>6814</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>78</v>
       </c>
@@ -1154,7 +1158,7 @@
         <v>6821</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>78</v>
       </c>
@@ -1174,7 +1178,7 @@
         <v>6820</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>74</v>
       </c>
@@ -1194,7 +1198,7 @@
         <v>6387</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>75</v>
       </c>
@@ -1214,7 +1218,7 @@
         <v>9883</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>78</v>
       </c>
@@ -1234,7 +1238,7 @@
         <v>8090</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>78</v>
       </c>
@@ -1254,7 +1258,7 @@
         <v>6753</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>74</v>
       </c>
@@ -1274,7 +1278,7 @@
         <v>9143</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>75</v>
       </c>
@@ -1294,7 +1298,7 @@
         <v>6366</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>74</v>
       </c>
@@ -1314,7 +1318,7 @@
         <v>8517</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>75</v>
       </c>
@@ -1334,7 +1338,7 @@
         <v>6359</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>74</v>
       </c>
@@ -1354,7 +1358,7 @@
         <v>6386</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>75</v>
       </c>
@@ -1374,7 +1378,7 @@
         <v>6641</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>74</v>
       </c>
@@ -1394,7 +1398,7 @@
         <v>8285</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>75</v>
       </c>
@@ -1414,7 +1418,7 @@
         <v>8149</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>78</v>
       </c>
@@ -1434,7 +1438,7 @@
         <v>6379</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>78</v>
       </c>
@@ -1454,7 +1458,7 @@
         <v>9085</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>74</v>
       </c>
@@ -1474,7 +1478,7 @@
         <v>8138</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>75</v>
       </c>
@@ -1494,7 +1498,7 @@
         <v>8136</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>77</v>
       </c>
@@ -1514,7 +1518,7 @@
         <v>8346</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>76</v>
       </c>
@@ -1534,7 +1538,7 @@
         <v>6627</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>77</v>
       </c>
@@ -1554,7 +1558,7 @@
         <v>8353</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>76</v>
       </c>
@@ -1574,7 +1578,7 @@
         <v>15500</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>77</v>
       </c>
@@ -1594,7 +1598,7 @@
         <v>8360</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>76</v>
       </c>
@@ -1614,7 +1618,7 @@
         <v>15498</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>77</v>
       </c>
@@ -1634,7 +1638,7 @@
         <v>8365</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>76</v>
       </c>
@@ -1654,7 +1658,7 @@
         <v>9898</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>77</v>
       </c>
@@ -1674,7 +1678,7 @@
         <v>8376</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>76</v>
       </c>
@@ -1694,7 +1698,7 @@
         <v>15443</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>77</v>
       </c>
@@ -1714,7 +1718,7 @@
         <v>7928</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>76</v>
       </c>
@@ -1743,19 +1747,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BB69EEE-758D-4994-98FD-EB06BA83BC9D}">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>69</v>
       </c>
@@ -1781,7 +1785,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>74</v>
       </c>
@@ -1807,7 +1811,7 @@
         <v>6392</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>75</v>
       </c>
@@ -1833,7 +1837,7 @@
         <v>6676</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>80</v>
       </c>
@@ -1859,7 +1863,7 @@
         <v>10225</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>79</v>
       </c>
@@ -1885,7 +1889,7 @@
         <v>8126</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>70</v>
       </c>
@@ -1911,7 +1915,7 @@
         <v>6668</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>71</v>
       </c>
@@ -1937,7 +1941,7 @@
         <v>5831</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>70</v>
       </c>
@@ -1963,7 +1967,7 @@
         <v>6542</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>71</v>
       </c>
@@ -1989,7 +1993,7 @@
         <v>5202</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>70</v>
       </c>
@@ -2015,7 +2019,7 @@
         <v>6511</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>71</v>
       </c>
@@ -2041,7 +2045,7 @@
         <v>5798</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>70</v>
       </c>
@@ -2067,7 +2071,7 @@
         <v>8155</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>71</v>
       </c>
@@ -2093,7 +2097,7 @@
         <v>7603</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>78</v>
       </c>
@@ -2117,6 +2121,11 @@
       </c>
       <c r="H14">
         <v>8341</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J16" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>